<commit_message>
update Data Table:  Examination type
</commit_message>
<xml_diff>
--- a/Acceptance Tests/Specialist.xlsx
+++ b/Acceptance Tests/Specialist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asaf/Desktop/GHealth-System/Acceptance Tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asaf/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="179">
   <si>
     <t xml:space="preserve">Use Case: </t>
   </si>
@@ -558,13 +558,37 @@
   </si>
   <si>
     <t>Electrocardiography</t>
+  </si>
+  <si>
+    <t>physiotherapy</t>
+  </si>
+  <si>
+    <t>Otorhinolaryngology</t>
+  </si>
+  <si>
+    <t>sinusitis</t>
+  </si>
+  <si>
+    <t>Hearing test</t>
+  </si>
+  <si>
+    <t>orthodontics</t>
+  </si>
+  <si>
+    <t>psoriasis</t>
+  </si>
+  <si>
+    <t>Tova</t>
+  </si>
+  <si>
+    <t>Papilloma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -618,6 +642,10 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -645,7 +673,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -861,12 +889,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1011,25 +1052,34 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1341,10 +1391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H96"/>
+  <dimension ref="A2:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="G90" sqref="G90"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="189" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2478,19 +2528,75 @@
       </c>
     </row>
     <row r="95" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="28" t="s">
+      <c r="A95" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="B95" s="42" t="s">
+      <c r="B95" s="59" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" s="58" t="s">
+      <c r="A96" s="60" t="s">
         <v>170</v>
       </c>
       <c r="B96" s="14" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="B97" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="58" t="s">
+        <v>178</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="58" t="s">
+        <v>173</v>
+      </c>
+      <c r="B99" s="57" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="58" t="s">
+        <v>174</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="58" t="s">
+        <v>175</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="61" t="s">
+        <v>177</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2521,8 +2627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2534,10 +2640,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="54"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -2663,10 +2769,10 @@
     </row>
     <row r="16" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="B17" s="53"/>
+      <c r="B17" s="54"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="26" t="s">
@@ -2704,7 +2810,7 @@
       </c>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
-      <c r="D23" s="54"/>
+      <c r="D23" s="52"/>
     </row>
     <row r="24" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
@@ -2720,17 +2826,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.2">
-      <c r="A25" s="56" t="s">
+    <row r="25" spans="1:4" ht="76" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="55" t="s">
         <v>162</v>
       </c>
-      <c r="B25" s="57" t="s">
+      <c r="B25" s="56" t="s">
         <v>165</v>
       </c>
-      <c r="C25" s="57" t="s">
+      <c r="C25" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="D25" s="55" t="s">
+      <c r="D25" s="10" t="s">
         <v>164</v>
       </c>
     </row>

</xml_diff>